<commit_message>
###STABLE### Fixed bug with PLAYER.MAP.LOCATION.LAST, which was masked and also causing a problem converting it to a screen hole.
</commit_message>
<xml_diff>
--- a/Map_Shapes/Map/2Map Objects.xlsx
+++ b/Map_Shapes/Map/2Map Objects.xlsx
@@ -125,7 +125,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="J23" authorId="0">
+    <comment ref="K17" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mark:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Used for detecting building-to-building enter/exits. This value is needed in byte 9 in addition to byte 1 because byte 0-8 aren't set in a building-to-building enter/exit so that when player exits the building location series, he will be returned to the entrance used on the surface map or undermap.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E23" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1786,7 +1810,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="328">
   <si>
     <t>Mobs (i.e. monsters)</t>
   </si>
@@ -2775,6 +2799,21 @@
   </si>
   <si>
     <t>DATA.MAP.M5</t>
+  </si>
+  <si>
+    <t>---------------</t>
+  </si>
+  <si>
+    <t>------------------------------------</t>
+  </si>
+  <si>
+    <t>------&gt;</t>
+  </si>
+  <si>
+    <t>(these used to be +$4 thru +$8)</t>
+  </si>
+  <si>
+    <t>(used to be +$9)</t>
   </si>
 </sst>
 </file>
@@ -3091,7 +3130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -3168,8 +3207,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -3177,6 +3214,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3476,8 +3517,8 @@
   </sheetPr>
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3497,22 +3538,22 @@
     <col min="13" max="13" width="32.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25">
+    <row r="1" spans="1:11" ht="23.25">
       <c r="D1" s="10" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:11">
       <c r="A6" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>60</v>
       </c>
@@ -3529,7 +3570,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>115</v>
       </c>
@@ -3546,17 +3587,17 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:11">
       <c r="F10" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:11">
       <c r="G11" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:11">
       <c r="A13" s="1" t="s">
         <v>109</v>
       </c>
@@ -3564,12 +3605,12 @@
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>60</v>
       </c>
@@ -3589,7 +3630,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
         <v>114</v>
       </c>
@@ -3607,12 +3648,18 @@
       </c>
       <c r="F16" t="s">
         <v>118</v>
+      </c>
+      <c r="K16" s="44" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" t="s">
         <v>119</v>
       </c>
+      <c r="K17" s="47" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" t="s">
@@ -3628,16 +3675,29 @@
       <c r="A20" s="1" t="s">
         <v>102</v>
       </c>
+      <c r="F20" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="21" spans="1:11">
-      <c r="E21" s="41" t="s">
+      <c r="E21" t="s">
+        <v>327</v>
+      </c>
+      <c r="F21" s="41" t="s">
         <v>292</v>
       </c>
-      <c r="F21" s="42"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="43"/>
+      <c r="G21" s="49" t="s">
+        <v>323</v>
+      </c>
+      <c r="H21" s="49" t="s">
+        <v>323</v>
+      </c>
+      <c r="I21" s="49" t="s">
+        <v>324</v>
+      </c>
+      <c r="J21" s="50" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" t="s">
@@ -3652,22 +3712,22 @@
       <c r="D22" t="s">
         <v>63</v>
       </c>
-      <c r="E22" s="44" t="s">
+      <c r="E22" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="F22" s="45" t="s">
+      <c r="F22" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="G22" s="45" t="s">
+      <c r="G22" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="H22" s="45" t="s">
+      <c r="H22" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="I22" s="45" t="s">
-        <v>106</v>
-      </c>
-      <c r="J22" s="46" t="s">
+      <c r="I22" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="J22" s="44" t="s">
         <v>145</v>
       </c>
     </row>
@@ -3684,30 +3744,30 @@
       <c r="D23" t="s">
         <v>99</v>
       </c>
-      <c r="E23" s="47" t="s">
+      <c r="E23" s="52" t="s">
+        <v>108</v>
+      </c>
+      <c r="F23" s="45" t="s">
         <v>103</v>
       </c>
-      <c r="F23" s="48" t="s">
+      <c r="G23" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="G23" s="48" t="s">
+      <c r="H23" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="H23" s="48" t="s">
+      <c r="I23" s="46" t="s">
         <v>101</v>
       </c>
-      <c r="I23" s="48" t="s">
+      <c r="J23" s="47" t="s">
         <v>105</v>
-      </c>
-      <c r="J23" s="49" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="B26" s="50" t="s">
+      <c r="B26" s="48" t="s">
         <v>317</v>
       </c>
       <c r="C26" s="37"/>
@@ -5979,7 +6039,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:M17"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
@@ -6166,8 +6226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:F85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7117,7 +7177,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>